<commit_message>
Implemented satisfaction criteria settings in Excel
</commit_message>
<xml_diff>
--- a/input/drivers.xlsx
+++ b/input/drivers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\thesis\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339601A4-1A20-4F6C-A8C4-1610FE9EAD2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B5F6C9-2A75-4324-82C0-CCCC03152F9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="15585" windowWidth="29040" windowHeight="15840" xr2:uid="{10EEE7EC-A4D0-4BC9-A599-2CBEC631D922}"/>
+    <workbookView xWindow="-23148" yWindow="12672" windowWidth="23256" windowHeight="12576" xr2:uid="{10EEE7EC-A4D0-4BC9-A599-2CBEC631D922}"/>
   </bookViews>
   <sheets>
     <sheet name="Internal drivers" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="163">
   <si>
     <t>Dummy</t>
   </si>
@@ -219,9 +219,6 @@
     <t>Bos, Joel</t>
   </si>
   <si>
-    <t>Sum</t>
-  </si>
-  <si>
     <t>Hotel stays</t>
   </si>
   <si>
@@ -249,12 +246,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Satisfaction criteria weights</t>
-  </si>
-  <si>
-    <t>Satisfaction criteria minimise/maximise</t>
-  </si>
-  <si>
     <t>Is optional?</t>
   </si>
   <si>
@@ -517,6 +508,24 @@
   </si>
   <si>
     <t>External driver name</t>
+  </si>
+  <si>
+    <t>(Sum)</t>
+  </si>
+  <si>
+    <t>Consecutive free days</t>
+  </si>
+  <si>
+    <t>Resting time</t>
+  </si>
+  <si>
+    <t>Time off requests</t>
+  </si>
+  <si>
+    <t>Satisfaction criterion weight</t>
+  </si>
+  <si>
+    <t>Satisfaction criterion mode</t>
   </si>
 </sst>
 </file>
@@ -560,7 +569,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -577,11 +586,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -928,10 +940,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6E05472-9174-4833-9EE7-2771F2F37981}">
-  <dimension ref="A1:T34"/>
+  <dimension ref="A1:W34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -942,100 +954,112 @@
     <col min="4" max="4" width="13.453125" style="1" customWidth="1"/>
     <col min="5" max="5" width="12.1796875" style="3" customWidth="1"/>
     <col min="6" max="10" width="12.08984375" style="1" customWidth="1"/>
-    <col min="11" max="19" width="12.08984375" style="2" customWidth="1"/>
-    <col min="20" max="20" width="28.453125" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="8.7265625" style="1"/>
+    <col min="11" max="22" width="12.08984375" style="2" customWidth="1"/>
+    <col min="23" max="23" width="28.453125" style="1" customWidth="1"/>
+    <col min="24" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="4" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D1" s="5" t="s">
+    <row r="1" spans="1:23" s="4" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="C1" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="6" t="s">
+      <c r="D1" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="5" t="s">
+      <c r="E1" s="7" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
+      <c r="F1" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
       <c r="F2" s="4" t="s">
         <v>67</v>
       </c>
       <c r="G2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="N2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="O2" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="Q2" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="K2" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>62</v>
-      </c>
       <c r="R2" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="S2" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="T2" s="5"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="S2" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="W2" s="7"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>59</v>
       </c>
@@ -1079,7 +1103,7 @@
         <v>0.05</v>
       </c>
       <c r="O3" s="2">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="P3" s="2">
         <v>0.05</v>
@@ -1091,11 +1115,20 @@
         <v>0.15</v>
       </c>
       <c r="S3" s="2">
-        <f>SUM(K3:R3)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="T3" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="U3" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="V3" s="2">
+        <f>SUM(K3:U3)</f>
+        <v>1.0000000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>57</v>
       </c>
@@ -1139,7 +1172,7 @@
         <v>0.05</v>
       </c>
       <c r="O4" s="2">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="P4" s="2">
         <v>0.05</v>
@@ -1151,11 +1184,20 @@
         <v>0.15</v>
       </c>
       <c r="S4" s="2">
-        <f>SUM(K4:R4)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="T4" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="U4" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="V4" s="2">
+        <f t="shared" ref="V4:V34" si="0">SUM(K4:U4)</f>
+        <v>1.0000000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>55</v>
       </c>
@@ -1199,7 +1241,7 @@
         <v>0.05</v>
       </c>
       <c r="O5" s="2">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="P5" s="2">
         <v>0.05</v>
@@ -1211,11 +1253,20 @@
         <v>0.15</v>
       </c>
       <c r="S5" s="2">
-        <f>SUM(K5:R5)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="T5" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="U5" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="V5" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>53</v>
       </c>
@@ -1259,7 +1310,7 @@
         <v>0.05</v>
       </c>
       <c r="O6" s="2">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="P6" s="2">
         <v>0.05</v>
@@ -1271,11 +1322,20 @@
         <v>0.15</v>
       </c>
       <c r="S6" s="2">
-        <f>SUM(K6:R6)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="T6" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="U6" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="V6" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>52</v>
       </c>
@@ -1319,7 +1379,7 @@
         <v>0.05</v>
       </c>
       <c r="O7" s="2">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="P7" s="2">
         <v>0.05</v>
@@ -1331,11 +1391,20 @@
         <v>0.15</v>
       </c>
       <c r="S7" s="2">
-        <f>SUM(K7:R7)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="T7" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="U7" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="V7" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>50</v>
       </c>
@@ -1379,7 +1448,7 @@
         <v>0.05</v>
       </c>
       <c r="O8" s="2">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="P8" s="2">
         <v>0.05</v>
@@ -1391,11 +1460,20 @@
         <v>0.15</v>
       </c>
       <c r="S8" s="2">
-        <f>SUM(K8:R8)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="T8" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="U8" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="V8" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>48</v>
       </c>
@@ -1439,7 +1517,7 @@
         <v>0.05</v>
       </c>
       <c r="O9" s="2">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="P9" s="2">
         <v>0.05</v>
@@ -1451,14 +1529,23 @@
         <v>0.15</v>
       </c>
       <c r="S9" s="2">
-        <f>SUM(K9:R9)</f>
-        <v>1</v>
-      </c>
-      <c r="T9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T9" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="U9" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="V9" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="W9" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>46</v>
       </c>
@@ -1502,7 +1589,7 @@
         <v>0.05</v>
       </c>
       <c r="O10" s="2">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="P10" s="2">
         <v>0.05</v>
@@ -1514,11 +1601,20 @@
         <v>0.15</v>
       </c>
       <c r="S10" s="2">
-        <f>SUM(K10:R10)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="T10" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="U10" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="V10" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>44</v>
       </c>
@@ -1562,7 +1658,7 @@
         <v>0.05</v>
       </c>
       <c r="O11" s="2">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="P11" s="2">
         <v>0.05</v>
@@ -1574,11 +1670,20 @@
         <v>0.15</v>
       </c>
       <c r="S11" s="2">
-        <f>SUM(K11:R11)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="T11" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="U11" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="V11" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>42</v>
       </c>
@@ -1622,7 +1727,7 @@
         <v>0.05</v>
       </c>
       <c r="O12" s="2">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="P12" s="2">
         <v>0.05</v>
@@ -1634,11 +1739,20 @@
         <v>0.15</v>
       </c>
       <c r="S12" s="2">
-        <f>SUM(K12:R12)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="T12" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="U12" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="V12" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>40</v>
       </c>
@@ -1682,7 +1796,7 @@
         <v>0.05</v>
       </c>
       <c r="O13" s="2">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="P13" s="2">
         <v>0.05</v>
@@ -1694,11 +1808,20 @@
         <v>0.15</v>
       </c>
       <c r="S13" s="2">
-        <f>SUM(K13:R13)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="T13" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="U13" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="V13" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>38</v>
       </c>
@@ -1742,7 +1865,7 @@
         <v>0.05</v>
       </c>
       <c r="O14" s="2">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="P14" s="2">
         <v>0.05</v>
@@ -1754,11 +1877,20 @@
         <v>0.15</v>
       </c>
       <c r="S14" s="2">
-        <f>SUM(K14:R14)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="T14" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="U14" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="V14" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>37</v>
       </c>
@@ -1802,7 +1934,7 @@
         <v>0.05</v>
       </c>
       <c r="O15" s="2">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="P15" s="2">
         <v>0.05</v>
@@ -1814,11 +1946,20 @@
         <v>0.15</v>
       </c>
       <c r="S15" s="2">
-        <f>SUM(K15:R15)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" ht="29" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="T15" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="U15" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="V15" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
@@ -1862,7 +2003,7 @@
         <v>0.05</v>
       </c>
       <c r="O16" s="2">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="P16" s="2">
         <v>0.05</v>
@@ -1874,14 +2015,23 @@
         <v>0.15</v>
       </c>
       <c r="S16" s="2">
-        <f>SUM(K16:R16)</f>
-        <v>1</v>
-      </c>
-      <c r="T16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T16" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="U16" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="V16" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="W16" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
@@ -1925,7 +2075,7 @@
         <v>0.05</v>
       </c>
       <c r="O17" s="2">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="P17" s="2">
         <v>0.05</v>
@@ -1937,11 +2087,20 @@
         <v>0.15</v>
       </c>
       <c r="S17" s="2">
-        <f>SUM(K17:R17)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="T17" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="U17" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="V17" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>30</v>
       </c>
@@ -1985,7 +2144,7 @@
         <v>0.05</v>
       </c>
       <c r="O18" s="2">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="P18" s="2">
         <v>0.05</v>
@@ -1997,14 +2156,23 @@
         <v>0.15</v>
       </c>
       <c r="S18" s="2">
-        <f>SUM(K18:R18)</f>
-        <v>1</v>
-      </c>
-      <c r="T18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T18" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="U18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="V18" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="W18" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>28</v>
       </c>
@@ -2048,7 +2216,7 @@
         <v>0.05</v>
       </c>
       <c r="O19" s="2">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="P19" s="2">
         <v>0.05</v>
@@ -2060,14 +2228,23 @@
         <v>0.15</v>
       </c>
       <c r="S19" s="2">
-        <f>SUM(K19:R19)</f>
-        <v>1</v>
-      </c>
-      <c r="T19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T19" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="U19" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="V19" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="W19" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>26</v>
       </c>
@@ -2111,7 +2288,7 @@
         <v>0.05</v>
       </c>
       <c r="O20" s="2">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="P20" s="2">
         <v>0.05</v>
@@ -2123,11 +2300,20 @@
         <v>0.15</v>
       </c>
       <c r="S20" s="2">
-        <f>SUM(K20:R20)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="T20" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="U20" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="V20" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -2171,7 +2357,7 @@
         <v>0.05</v>
       </c>
       <c r="O21" s="2">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="P21" s="2">
         <v>0.05</v>
@@ -2183,11 +2369,20 @@
         <v>0.15</v>
       </c>
       <c r="S21" s="2">
-        <f>SUM(K21:R21)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="T21" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="U21" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="V21" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -2231,7 +2426,7 @@
         <v>0.05</v>
       </c>
       <c r="O22" s="2">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="P22" s="2">
         <v>0.05</v>
@@ -2243,11 +2438,20 @@
         <v>0.15</v>
       </c>
       <c r="S22" s="2">
-        <f>SUM(K22:R22)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="T22" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="U22" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="V22" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
@@ -2291,7 +2495,7 @@
         <v>0.05</v>
       </c>
       <c r="O23" s="2">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="P23" s="2">
         <v>0.05</v>
@@ -2303,14 +2507,23 @@
         <v>0.15</v>
       </c>
       <c r="S23" s="2">
-        <f>SUM(K23:R23)</f>
-        <v>1</v>
-      </c>
-      <c r="T23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T23" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="U23" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="V23" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="W23" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>16</v>
       </c>
@@ -2354,7 +2567,7 @@
         <v>0.05</v>
       </c>
       <c r="O24" s="2">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="P24" s="2">
         <v>0.05</v>
@@ -2366,11 +2579,20 @@
         <v>0.15</v>
       </c>
       <c r="S24" s="2">
-        <f>SUM(K24:R24)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="T24" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="U24" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="V24" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>13</v>
       </c>
@@ -2414,7 +2636,7 @@
         <v>0.05</v>
       </c>
       <c r="O25" s="2">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="P25" s="2">
         <v>0.05</v>
@@ -2426,14 +2648,23 @@
         <v>0.15</v>
       </c>
       <c r="S25" s="2">
-        <f>SUM(K25:R25)</f>
-        <v>1</v>
-      </c>
-      <c r="T25" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="T25" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="U25" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="V25" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="W25" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>12</v>
       </c>
@@ -2477,7 +2708,7 @@
         <v>0.05</v>
       </c>
       <c r="O26" s="2">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="P26" s="2">
         <v>0.05</v>
@@ -2489,14 +2720,23 @@
         <v>0.15</v>
       </c>
       <c r="S26" s="2">
-        <f>SUM(K26:R26)</f>
-        <v>1</v>
-      </c>
-      <c r="T26" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="T26" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="U26" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="V26" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="W26" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>11</v>
       </c>
@@ -2540,7 +2780,7 @@
         <v>0.05</v>
       </c>
       <c r="O27" s="2">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="P27" s="2">
         <v>0.05</v>
@@ -2552,14 +2792,23 @@
         <v>0.15</v>
       </c>
       <c r="S27" s="2">
-        <f>SUM(K27:R27)</f>
-        <v>1</v>
-      </c>
-      <c r="T27" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="T27" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="U27" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="V27" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="W27" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>10</v>
       </c>
@@ -2603,7 +2852,7 @@
         <v>0.05</v>
       </c>
       <c r="O28" s="2">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="P28" s="2">
         <v>0.05</v>
@@ -2615,14 +2864,23 @@
         <v>0.15</v>
       </c>
       <c r="S28" s="2">
-        <f>SUM(K28:R28)</f>
-        <v>1</v>
-      </c>
-      <c r="T28" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="T28" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="U28" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="V28" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="W28" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>9</v>
       </c>
@@ -2666,7 +2924,7 @@
         <v>0.05</v>
       </c>
       <c r="O29" s="2">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="P29" s="2">
         <v>0.05</v>
@@ -2678,14 +2936,23 @@
         <v>0.15</v>
       </c>
       <c r="S29" s="2">
-        <f>SUM(K29:R29)</f>
-        <v>1</v>
-      </c>
-      <c r="T29" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="T29" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="U29" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="V29" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="W29" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>8</v>
       </c>
@@ -2729,7 +2996,7 @@
         <v>0.05</v>
       </c>
       <c r="O30" s="2">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="P30" s="2">
         <v>0.05</v>
@@ -2741,14 +3008,23 @@
         <v>0.15</v>
       </c>
       <c r="S30" s="2">
-        <f>SUM(K30:R30)</f>
-        <v>1</v>
-      </c>
-      <c r="T30" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="T30" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="U30" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="V30" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="W30" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>7</v>
       </c>
@@ -2792,7 +3068,7 @@
         <v>0.05</v>
       </c>
       <c r="O31" s="2">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="P31" s="2">
         <v>0.05</v>
@@ -2804,14 +3080,23 @@
         <v>0.15</v>
       </c>
       <c r="S31" s="2">
-        <f>SUM(K31:R31)</f>
-        <v>1</v>
-      </c>
-      <c r="T31" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="T31" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="U31" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="V31" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="W31" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>6</v>
       </c>
@@ -2855,7 +3140,7 @@
         <v>0.05</v>
       </c>
       <c r="O32" s="2">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="P32" s="2">
         <v>0.05</v>
@@ -2867,14 +3152,23 @@
         <v>0.15</v>
       </c>
       <c r="S32" s="2">
-        <f>SUM(K32:R32)</f>
-        <v>1</v>
-      </c>
-      <c r="T32" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="T32" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="U32" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="V32" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="W32" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>5</v>
       </c>
@@ -2918,7 +3212,7 @@
         <v>0.05</v>
       </c>
       <c r="O33" s="2">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="P33" s="2">
         <v>0.05</v>
@@ -2930,14 +3224,23 @@
         <v>0.15</v>
       </c>
       <c r="S33" s="2">
-        <f>SUM(K33:R33)</f>
-        <v>1</v>
-      </c>
-      <c r="T33" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="T33" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="U33" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="V33" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="W33" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>4</v>
       </c>
@@ -2981,7 +3284,7 @@
         <v>0.05</v>
       </c>
       <c r="O34" s="2">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="P34" s="2">
         <v>0.05</v>
@@ -2993,10 +3296,19 @@
         <v>0.15</v>
       </c>
       <c r="S34" s="2">
-        <f>SUM(K34:R34)</f>
-        <v>1</v>
-      </c>
-      <c r="T34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T34" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="U34" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="V34" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="W34" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3006,38 +3318,13 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="W1:W2"/>
     <mergeCell ref="F1:J1"/>
-    <mergeCell ref="K1:S1"/>
+    <mergeCell ref="K1:V1"/>
     <mergeCell ref="E1:E2"/>
   </mergeCells>
-  <conditionalFormatting sqref="S3:S25 S35:S1048576">
+  <conditionalFormatting sqref="V3:V1048576">
     <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S26">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S27:S29">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S30">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S31">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S32:S34">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3062,35 +3349,35 @@
     <col min="8" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="E1" s="7" t="s">
+    <row r="1" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="C1" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>97</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>15</v>
@@ -3105,15 +3392,15 @@
         <v>15</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>25</v>
@@ -3128,15 +3415,15 @@
         <v>4</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>15</v>
@@ -3151,15 +3438,15 @@
         <v>12</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>25</v>
@@ -3174,15 +3461,15 @@
         <v>7</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>15</v>
@@ -3197,15 +3484,15 @@
         <v>18</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>15</v>
@@ -3220,15 +3507,15 @@
         <v>6</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B8" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>25</v>
@@ -3243,15 +3530,15 @@
         <v>6</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>15</v>
@@ -3266,15 +3553,15 @@
         <v>0</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>25</v>
@@ -3289,15 +3576,15 @@
         <v>0</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>3</v>
@@ -3317,10 +3604,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>25</v>
@@ -3359,22 +3646,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>157</v>
+      <c r="A1" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C2" s="1" t="b">
         <v>0</v>
@@ -3382,10 +3669,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C3" s="1" t="b">
         <v>0</v>
@@ -3393,10 +3680,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C4" s="1" t="b">
         <v>0</v>
@@ -3404,10 +3691,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C5" s="1" t="b">
         <v>0</v>
@@ -3415,10 +3702,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C6" s="1" t="b">
         <v>0</v>
@@ -3426,10 +3713,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C7" s="1" t="b">
         <v>0</v>
@@ -3437,10 +3724,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C8" s="1" t="b">
         <v>1</v>
@@ -3448,10 +3735,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C9" s="1" t="b">
         <v>1</v>
@@ -3459,10 +3746,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C10" s="1" t="b">
         <v>0</v>
@@ -3470,10 +3757,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C11" s="1" t="b">
         <v>0</v>
@@ -3481,10 +3768,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C12" s="1" t="b">
         <v>0</v>
@@ -3492,10 +3779,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C13" s="1" t="b">
         <v>0</v>
@@ -3503,10 +3790,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C14" s="1" t="b">
         <v>0</v>
@@ -3514,10 +3801,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C15" s="1" t="b">
         <v>0</v>
@@ -3525,10 +3812,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C16" s="1" t="b">
         <v>0</v>
@@ -3536,10 +3823,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C17" s="1" t="b">
         <v>0</v>
@@ -3547,10 +3834,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C18" s="1" t="b">
         <v>0</v>
@@ -3558,10 +3845,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C19" s="1" t="b">
         <v>0</v>
@@ -3569,10 +3856,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B20" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C20" s="1" t="b">
         <v>1</v>
@@ -3580,10 +3867,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C21" s="1" t="b">
         <v>0</v>
@@ -3591,10 +3878,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C22" s="1" t="b">
         <v>0</v>
@@ -3602,10 +3889,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C23" s="1" t="b">
         <v>0</v>
@@ -3613,10 +3900,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C24" s="1" t="b">
         <v>0</v>
@@ -3624,10 +3911,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C25" s="1" t="b">
         <v>1</v>
@@ -3635,10 +3922,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C26" s="1" t="b">
         <v>0</v>
@@ -3646,10 +3933,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C27" s="1" t="b">
         <v>1</v>
@@ -3657,10 +3944,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C28" s="1" t="b">
         <v>0</v>
@@ -3668,10 +3955,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C29" s="1" t="b">
         <v>0</v>
@@ -3679,10 +3966,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C30" s="1" t="b">
         <v>0</v>
@@ -3690,10 +3977,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C31" s="1" t="b">
         <v>0</v>
@@ -3701,10 +3988,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C32" s="1" t="b">
         <v>0</v>
@@ -3712,10 +3999,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C33" s="1" t="b">
         <v>0</v>
@@ -3723,10 +4010,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C34" s="1" t="b">
         <v>0</v>
@@ -3734,10 +4021,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C35" s="1" t="b">
         <v>0</v>
@@ -3745,10 +4032,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C36" s="1" t="b">
         <v>0</v>
@@ -3756,10 +4043,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C37" s="1" t="b">
         <v>0</v>
@@ -3767,10 +4054,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C38" s="1" t="b">
         <v>0</v>
@@ -3778,10 +4065,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C39" s="1" t="b">
         <v>0</v>
@@ -3789,10 +4076,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C40" s="1" t="b">
         <v>1</v>
@@ -3800,10 +4087,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C41" s="1" t="b">
         <v>0</v>
@@ -3811,10 +4098,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C42" s="1" t="b">
         <v>0</v>
@@ -3822,10 +4109,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C43" s="1" t="b">
         <v>0</v>
@@ -3833,10 +4120,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C44" s="1" t="b">
         <v>0</v>
@@ -3844,10 +4131,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C45" s="1" t="b">
         <v>0</v>
@@ -3855,10 +4142,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C46" s="1" t="b">
         <v>0</v>
@@ -3866,10 +4153,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C47" s="1" t="b">
         <v>0</v>
@@ -3877,10 +4164,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C48" s="1" t="b">
         <v>0</v>
@@ -3888,10 +4175,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C49" s="1" t="b">
         <v>0</v>
@@ -3899,10 +4186,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C50" s="1" t="b">
         <v>0</v>
@@ -3910,10 +4197,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C51" s="1" t="b">
         <v>0</v>
@@ -3921,10 +4208,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C52" s="1" t="b">
         <v>0</v>
@@ -3932,10 +4219,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C53" s="1" t="b">
         <v>0</v>
@@ -3943,10 +4230,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C54" s="1" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Bugfix to satisfaction criteria settings
</commit_message>
<xml_diff>
--- a/input/drivers.xlsx
+++ b/input/drivers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\thesis\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B5F6C9-2A75-4324-82C0-CCCC03152F9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956AB644-027D-4424-BB23-AE8A137B5E1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="12672" windowWidth="23256" windowHeight="12576" xr2:uid="{10EEE7EC-A4D0-4BC9-A599-2CBEC631D922}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="164">
   <si>
     <t>Dummy</t>
   </si>
@@ -526,6 +526,9 @@
   </si>
   <si>
     <t>Satisfaction criterion mode</t>
+  </si>
+  <si>
+    <t>Maximise</t>
   </si>
 </sst>
 </file>
@@ -599,32 +602,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -943,7 +921,7 @@
   <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1076,7 +1054,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>1</v>
@@ -1145,7 +1123,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>1</v>
@@ -1214,7 +1192,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>1</v>
@@ -1283,7 +1261,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>1</v>
@@ -1352,7 +1330,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>1</v>
@@ -1421,7 +1399,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>1</v>
@@ -1490,7 +1468,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>1</v>
@@ -1562,7 +1540,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>1</v>
@@ -1631,7 +1609,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>1</v>
@@ -1700,7 +1678,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>1</v>
@@ -1769,7 +1747,7 @@
         <v>0</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>1</v>
@@ -1838,7 +1816,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>1</v>
@@ -1907,7 +1885,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>1</v>
@@ -1976,7 +1954,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>1</v>
@@ -2048,7 +2026,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>1</v>
@@ -2117,7 +2095,7 @@
         <v>0</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>1</v>
@@ -2189,7 +2167,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>1</v>
@@ -2261,7 +2239,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>1</v>
@@ -2330,7 +2308,7 @@
         <v>0</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>1</v>
@@ -2399,7 +2377,7 @@
         <v>0</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>1</v>
@@ -2468,7 +2446,7 @@
         <v>0</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>1</v>
@@ -2540,7 +2518,7 @@
         <v>0</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>1</v>
@@ -2609,7 +2587,7 @@
         <v>1</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>1</v>
@@ -2681,7 +2659,7 @@
         <v>1</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>1</v>
@@ -2753,7 +2731,7 @@
         <v>1</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>1</v>
@@ -2825,7 +2803,7 @@
         <v>1</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>1</v>
@@ -2897,7 +2875,7 @@
         <v>1</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>1</v>
@@ -2969,7 +2947,7 @@
         <v>1</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>1</v>
@@ -3041,7 +3019,7 @@
         <v>1</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>1</v>
@@ -3113,7 +3091,7 @@
         <v>1</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>1</v>
@@ -3185,7 +3163,7 @@
         <v>1</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>1</v>
@@ -3257,7 +3235,7 @@
         <v>1</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>1</v>
@@ -3324,7 +3302,7 @@
     <mergeCell ref="E1:E2"/>
   </mergeCells>
   <conditionalFormatting sqref="V3:V1048576">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Started implementing availability (WIP)
</commit_message>
<xml_diff>
--- a/input/drivers.xlsx
+++ b/input/drivers.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\thesis\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956AB644-027D-4424-BB23-AE8A137B5E1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638F84F5-0F15-4A98-87CA-29F8E63C14AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="12672" windowWidth="23256" windowHeight="12576" xr2:uid="{10EEE7EC-A4D0-4BC9-A599-2CBEC631D922}"/>
+    <workbookView xWindow="-23148" yWindow="12672" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{10EEE7EC-A4D0-4BC9-A599-2CBEC631D922}"/>
   </bookViews>
   <sheets>
     <sheet name="Internal drivers" sheetId="2" r:id="rId1"/>
-    <sheet name="External driver companies" sheetId="3" r:id="rId2"/>
-    <sheet name="External drivers" sheetId="4" r:id="rId3"/>
+    <sheet name="Internal driver unavailability" sheetId="5" r:id="rId2"/>
+    <sheet name="External driver companies" sheetId="3" r:id="rId3"/>
+    <sheet name="External drivers" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="169">
   <si>
     <t>Dummy</t>
   </si>
@@ -519,9 +520,6 @@
     <t>Resting time</t>
   </si>
   <si>
-    <t>Time off requests</t>
-  </si>
-  <si>
     <t>Satisfaction criterion weight</t>
   </si>
   <si>
@@ -529,6 +527,24 @@
   </si>
   <si>
     <t>Maximise</t>
+  </si>
+  <si>
+    <t>Unavailable from</t>
+  </si>
+  <si>
+    <t>Unavailable until</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Hour</t>
+  </si>
+  <si>
+    <t>Unavailable on Monday</t>
+  </si>
+  <si>
+    <t>Unavailable on Wednesday 12:00-18:00</t>
   </si>
 </sst>
 </file>
@@ -572,7 +588,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -597,6 +613,12 @@
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -918,10 +940,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6E05472-9174-4833-9EE7-2771F2F37981}">
-  <dimension ref="A1:W34"/>
+  <dimension ref="A1:V34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -932,12 +954,12 @@
     <col min="4" max="4" width="13.453125" style="1" customWidth="1"/>
     <col min="5" max="5" width="12.1796875" style="3" customWidth="1"/>
     <col min="6" max="10" width="12.08984375" style="1" customWidth="1"/>
-    <col min="11" max="22" width="12.08984375" style="2" customWidth="1"/>
-    <col min="23" max="23" width="28.453125" style="1" customWidth="1"/>
-    <col min="24" max="16384" width="8.7265625" style="1"/>
+    <col min="11" max="21" width="12.08984375" style="2" customWidth="1"/>
+    <col min="22" max="22" width="28.453125" style="1" customWidth="1"/>
+    <col min="23" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="4" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" s="4" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>73</v>
       </c>
@@ -954,14 +976,14 @@
         <v>69</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
       <c r="K1" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L1" s="8"/>
       <c r="M1" s="8"/>
@@ -973,12 +995,11 @@
       <c r="S1" s="8"/>
       <c r="T1" s="8"/>
       <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
-      <c r="W1" s="7" t="s">
+      <c r="V1" s="7" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:23" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -1024,20 +1045,17 @@
         <v>60</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="T2" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="U2" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="U2" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="W2" s="7"/>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="V2" s="7"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>59</v>
       </c>
@@ -1054,7 +1072,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>1</v>
@@ -1093,20 +1111,17 @@
         <v>0.15</v>
       </c>
       <c r="S3" s="2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="T3" s="2">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="U3" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="V3" s="2">
-        <f>SUM(K3:U3)</f>
+        <f>SUM(K3:T3)</f>
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>57</v>
       </c>
@@ -1123,7 +1138,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>1</v>
@@ -1162,20 +1177,17 @@
         <v>0.15</v>
       </c>
       <c r="S4" s="2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="T4" s="2">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="U4" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="V4" s="2">
-        <f t="shared" ref="V4:V34" si="0">SUM(K4:U4)</f>
+        <f t="shared" ref="U4:U34" si="0">SUM(K4:T4)</f>
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>55</v>
       </c>
@@ -1192,7 +1204,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>1</v>
@@ -1231,20 +1243,17 @@
         <v>0.15</v>
       </c>
       <c r="S5" s="2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="T5" s="2">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="U5" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="V5" s="2">
         <f t="shared" si="0"/>
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>53</v>
       </c>
@@ -1261,7 +1270,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>1</v>
@@ -1300,20 +1309,17 @@
         <v>0.15</v>
       </c>
       <c r="S6" s="2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="T6" s="2">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="U6" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="V6" s="2">
         <f t="shared" si="0"/>
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>52</v>
       </c>
@@ -1330,7 +1336,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>1</v>
@@ -1369,20 +1375,17 @@
         <v>0.15</v>
       </c>
       <c r="S7" s="2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="T7" s="2">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="U7" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="V7" s="2">
         <f t="shared" si="0"/>
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>50</v>
       </c>
@@ -1399,7 +1402,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>1</v>
@@ -1438,20 +1441,17 @@
         <v>0.15</v>
       </c>
       <c r="S8" s="2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="T8" s="2">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="U8" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="V8" s="2">
         <f t="shared" si="0"/>
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>48</v>
       </c>
@@ -1468,7 +1468,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>1</v>
@@ -1507,23 +1507,20 @@
         <v>0.15</v>
       </c>
       <c r="S9" s="2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="T9" s="2">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="U9" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="V9" s="2">
         <f t="shared" si="0"/>
         <v>1.0000000000000002</v>
       </c>
-      <c r="W9" s="1" t="s">
+      <c r="V9" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>46</v>
       </c>
@@ -1540,7 +1537,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>1</v>
@@ -1579,20 +1576,17 @@
         <v>0.15</v>
       </c>
       <c r="S10" s="2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="T10" s="2">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="U10" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="V10" s="2">
         <f t="shared" si="0"/>
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>44</v>
       </c>
@@ -1609,7 +1603,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>1</v>
@@ -1648,20 +1642,17 @@
         <v>0.15</v>
       </c>
       <c r="S11" s="2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="T11" s="2">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="U11" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="V11" s="2">
         <f t="shared" si="0"/>
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>42</v>
       </c>
@@ -1678,7 +1669,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>1</v>
@@ -1717,20 +1708,17 @@
         <v>0.15</v>
       </c>
       <c r="S12" s="2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="T12" s="2">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="U12" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="V12" s="2">
         <f t="shared" si="0"/>
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>40</v>
       </c>
@@ -1747,7 +1735,7 @@
         <v>0</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>1</v>
@@ -1786,20 +1774,17 @@
         <v>0.15</v>
       </c>
       <c r="S13" s="2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="T13" s="2">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="U13" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="V13" s="2">
         <f t="shared" si="0"/>
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>38</v>
       </c>
@@ -1816,7 +1801,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>1</v>
@@ -1855,20 +1840,17 @@
         <v>0.15</v>
       </c>
       <c r="S14" s="2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="T14" s="2">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="U14" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="V14" s="2">
         <f t="shared" si="0"/>
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>37</v>
       </c>
@@ -1885,7 +1867,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>1</v>
@@ -1924,20 +1906,17 @@
         <v>0.15</v>
       </c>
       <c r="S15" s="2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="T15" s="2">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="U15" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="V15" s="2">
         <f t="shared" si="0"/>
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:23" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
@@ -1954,7 +1933,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>1</v>
@@ -1993,23 +1972,20 @@
         <v>0.15</v>
       </c>
       <c r="S16" s="2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="T16" s="2">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="U16" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="V16" s="2">
         <f t="shared" si="0"/>
         <v>1.0000000000000002</v>
       </c>
-      <c r="W16" s="1" t="s">
+      <c r="V16" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
@@ -2026,7 +2002,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>1</v>
@@ -2065,20 +2041,17 @@
         <v>0.15</v>
       </c>
       <c r="S17" s="2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="T17" s="2">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="U17" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="V17" s="2">
         <f t="shared" si="0"/>
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>30</v>
       </c>
@@ -2095,7 +2068,7 @@
         <v>0</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>1</v>
@@ -2134,23 +2107,20 @@
         <v>0.15</v>
       </c>
       <c r="S18" s="2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="T18" s="2">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="U18" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="V18" s="2">
         <f t="shared" si="0"/>
         <v>1.0000000000000002</v>
       </c>
-      <c r="W18" s="1" t="s">
+      <c r="V18" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>28</v>
       </c>
@@ -2167,7 +2137,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>1</v>
@@ -2206,23 +2176,20 @@
         <v>0.15</v>
       </c>
       <c r="S19" s="2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="T19" s="2">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="U19" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="V19" s="2">
         <f t="shared" si="0"/>
         <v>1.0000000000000002</v>
       </c>
-      <c r="W19" s="1" t="s">
+      <c r="V19" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>26</v>
       </c>
@@ -2239,7 +2206,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>1</v>
@@ -2278,20 +2245,17 @@
         <v>0.15</v>
       </c>
       <c r="S20" s="2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="T20" s="2">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="U20" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="V20" s="2">
         <f t="shared" si="0"/>
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -2308,7 +2272,7 @@
         <v>0</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>1</v>
@@ -2347,20 +2311,17 @@
         <v>0.15</v>
       </c>
       <c r="S21" s="2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="T21" s="2">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="U21" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="V21" s="2">
         <f t="shared" si="0"/>
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -2377,7 +2338,7 @@
         <v>0</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>1</v>
@@ -2416,20 +2377,17 @@
         <v>0.15</v>
       </c>
       <c r="S22" s="2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="T22" s="2">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="U22" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="V22" s="2">
         <f t="shared" si="0"/>
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
@@ -2446,7 +2404,7 @@
         <v>0</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>1</v>
@@ -2485,23 +2443,20 @@
         <v>0.15</v>
       </c>
       <c r="S23" s="2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="T23" s="2">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="U23" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="V23" s="2">
         <f t="shared" si="0"/>
         <v>1.0000000000000002</v>
       </c>
-      <c r="W23" s="1" t="s">
+      <c r="V23" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>16</v>
       </c>
@@ -2518,7 +2473,7 @@
         <v>0</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>1</v>
@@ -2557,20 +2512,17 @@
         <v>0.15</v>
       </c>
       <c r="S24" s="2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="T24" s="2">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="U24" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="V24" s="2">
         <f t="shared" si="0"/>
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>13</v>
       </c>
@@ -2587,7 +2539,7 @@
         <v>1</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>1</v>
@@ -2626,23 +2578,20 @@
         <v>0.15</v>
       </c>
       <c r="S25" s="2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="T25" s="2">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="U25" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="V25" s="2">
         <f t="shared" si="0"/>
         <v>1.0000000000000002</v>
       </c>
-      <c r="W25" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="V25" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>12</v>
       </c>
@@ -2659,7 +2608,7 @@
         <v>1</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>1</v>
@@ -2698,23 +2647,20 @@
         <v>0.15</v>
       </c>
       <c r="S26" s="2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="T26" s="2">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="U26" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="V26" s="2">
         <f t="shared" si="0"/>
         <v>1.0000000000000002</v>
       </c>
-      <c r="W26" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="V26" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>11</v>
       </c>
@@ -2731,7 +2677,7 @@
         <v>1</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>1</v>
@@ -2770,23 +2716,20 @@
         <v>0.15</v>
       </c>
       <c r="S27" s="2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="T27" s="2">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="U27" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="V27" s="2">
         <f t="shared" si="0"/>
         <v>1.0000000000000002</v>
       </c>
-      <c r="W27" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="V27" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>10</v>
       </c>
@@ -2803,7 +2746,7 @@
         <v>1</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>1</v>
@@ -2842,23 +2785,20 @@
         <v>0.15</v>
       </c>
       <c r="S28" s="2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="T28" s="2">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="U28" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="V28" s="2">
         <f t="shared" si="0"/>
         <v>1.0000000000000002</v>
       </c>
-      <c r="W28" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="V28" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>9</v>
       </c>
@@ -2875,7 +2815,7 @@
         <v>1</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>1</v>
@@ -2914,23 +2854,20 @@
         <v>0.15</v>
       </c>
       <c r="S29" s="2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="T29" s="2">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="U29" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="V29" s="2">
         <f t="shared" si="0"/>
         <v>1.0000000000000002</v>
       </c>
-      <c r="W29" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="V29" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>8</v>
       </c>
@@ -2947,7 +2884,7 @@
         <v>1</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>1</v>
@@ -2986,23 +2923,20 @@
         <v>0.15</v>
       </c>
       <c r="S30" s="2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="T30" s="2">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="U30" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="V30" s="2">
         <f t="shared" si="0"/>
         <v>1.0000000000000002</v>
       </c>
-      <c r="W30" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="V30" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>7</v>
       </c>
@@ -3019,7 +2953,7 @@
         <v>1</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>1</v>
@@ -3058,23 +2992,20 @@
         <v>0.15</v>
       </c>
       <c r="S31" s="2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="T31" s="2">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="U31" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="V31" s="2">
         <f t="shared" si="0"/>
         <v>1.0000000000000002</v>
       </c>
-      <c r="W31" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="V31" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>6</v>
       </c>
@@ -3091,7 +3022,7 @@
         <v>1</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>1</v>
@@ -3130,23 +3061,20 @@
         <v>0.15</v>
       </c>
       <c r="S32" s="2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="T32" s="2">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="U32" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="V32" s="2">
         <f t="shared" si="0"/>
         <v>1.0000000000000002</v>
       </c>
-      <c r="W32" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="V32" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>5</v>
       </c>
@@ -3163,7 +3091,7 @@
         <v>1</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>1</v>
@@ -3202,23 +3130,20 @@
         <v>0.15</v>
       </c>
       <c r="S33" s="2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="T33" s="2">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="U33" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="V33" s="2">
         <f t="shared" si="0"/>
         <v>1.0000000000000002</v>
       </c>
-      <c r="W33" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="V33" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>4</v>
       </c>
@@ -3235,7 +3160,7 @@
         <v>1</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>1</v>
@@ -3274,19 +3199,16 @@
         <v>0.15</v>
       </c>
       <c r="S34" s="2">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="T34" s="2">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="U34" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="V34" s="2">
         <f t="shared" si="0"/>
         <v>1.0000000000000002</v>
       </c>
-      <c r="W34" s="1" t="s">
+      <c r="V34" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3296,12 +3218,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="W1:W2"/>
+    <mergeCell ref="V1:V2"/>
     <mergeCell ref="F1:J1"/>
-    <mergeCell ref="K1:V1"/>
+    <mergeCell ref="K1:U1"/>
     <mergeCell ref="E1:E2"/>
   </mergeCells>
-  <conditionalFormatting sqref="V3:V1048576">
+  <conditionalFormatting sqref="U3:U1048576">
     <cfRule type="cellIs" dxfId="0" priority="6" operator="lessThan">
       <formula>1</formula>
     </cfRule>
@@ -3312,6 +3234,106 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75027BDD-1E0A-47DF-BA10-0E624BCD9BEB}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="21.1796875" style="1" customWidth="1"/>
+    <col min="2" max="5" width="11.26953125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="42.1796875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.7265625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="7"/>
+      <c r="B2" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="F2" s="9"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>24</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1">
+        <v>18</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:F2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1181BC34-3767-4F68-BC10-33168BEF740B}">
   <dimension ref="A1:G12"/>
   <sheetViews>
@@ -3608,7 +3630,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0CCEFC9-8926-4B29-82BD-613C0CA7FAF4}">
   <dimension ref="A1:C54"/>
   <sheetViews>

</xml_diff>

<commit_message>
Properly implemented driver availability
</commit_message>
<xml_diff>
--- a/input/drivers.xlsx
+++ b/input/drivers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\thesis\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\thesis\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638F84F5-0F15-4A98-87CA-29F8E63C14AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4265DB23-3BF0-434E-810D-F401EE58277F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="12672" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{10EEE7EC-A4D0-4BC9-A599-2CBEC631D922}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{10EEE7EC-A4D0-4BC9-A599-2CBEC631D922}"/>
   </bookViews>
   <sheets>
     <sheet name="Internal drivers" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="167">
   <si>
     <t>Dummy</t>
   </si>
@@ -539,12 +538,6 @@
   </si>
   <si>
     <t>Hour</t>
-  </si>
-  <si>
-    <t>Unavailable on Monday</t>
-  </si>
-  <si>
-    <t>Unavailable on Wednesday 12:00-18:00</t>
   </si>
 </sst>
 </file>
@@ -609,13 +602,13 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -943,7 +936,7 @@
   <dimension ref="A1:V34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A5" sqref="A5:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -960,51 +953,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="4" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="8" t="s">
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="7" t="s">
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="8" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:22" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
       <c r="F2" s="4" t="s">
         <v>67</v>
       </c>
@@ -1053,7 +1046,7 @@
       <c r="U2" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="V2" s="7"/>
+      <c r="V2" s="8"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
@@ -3235,10 +3228,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75027BDD-1E0A-47DF-BA10-0E624BCD9BEB}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="F8" sqref="A3:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3249,77 +3242,37 @@
     <col min="7" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9" t="s">
+      <c r="E1" s="10"/>
+      <c r="F1" s="10" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="7"/>
-      <c r="B2" s="10" t="s">
+    <row r="2" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="8"/>
+      <c r="B2" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="F2" s="9"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1">
-        <v>24</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" s="1">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1">
-        <v>12</v>
-      </c>
-      <c r="D4" s="1">
-        <v>3</v>
-      </c>
-      <c r="E4" s="1">
-        <v>18</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>168</v>
-      </c>
+      <c r="F2" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Improved travel info usability
</commit_message>
<xml_diff>
--- a/input/drivers.xlsx
+++ b/input/drivers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\thesis\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4265DB23-3BF0-434E-810D-F401EE58277F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A845D895-7D21-4CF8-B52B-762D6A069387}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{10EEE7EC-A4D0-4BC9-A599-2CBEC631D922}"/>
+    <workbookView xWindow="-23148" yWindow="12804" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{10EEE7EC-A4D0-4BC9-A599-2CBEC631D922}"/>
   </bookViews>
   <sheets>
     <sheet name="Internal drivers" sheetId="2" r:id="rId1"/>
@@ -3230,8 +3230,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75027BDD-1E0A-47DF-BA10-0E624BCD9BEB}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="A3:F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3587,8 +3587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0CCEFC9-8926-4B29-82BD-613C0CA7FAF4}">
   <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>